<commit_message>
This is a message
</commit_message>
<xml_diff>
--- a/11MIAR_10_A_2024-25_CF - Herramientas de Estadística/Actividad 1/datos_inf.xlsx
+++ b/11MIAR_10_A_2024-25_CF - Herramientas de Estadística/Actividad 1/datos_inf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/walterandresortizvargas/Desktop/escritorio/VIU/VIU 2023/E1-2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\vui_master_202410\11MIAR_10_A_2024-25_CF - Herramientas de Estadística\Actividad 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31134D67-E6C4-C941-80BA-6D1781DEEA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023F59DB-1E32-48D4-AF51-0BE845B5B66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15600" xr2:uid="{3A6E57D2-D10B-F547-9703-4AD24FC555A1}"/>
+    <workbookView xWindow="4350" yWindow="2115" windowWidth="21600" windowHeight="11385" xr2:uid="{3A6E57D2-D10B-F547-9703-4AD24FC555A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -145,7 +145,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -251,7 +251,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -393,7 +393,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -403,16 +403,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4185AE9-FDA7-BB43-8135-BE84179D36C5}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>80.242999999999995</v>
       </c>
@@ -452,7 +450,7 @@
         <v>69.710999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>66.472999999999999</v>
       </c>
@@ -472,7 +470,7 @@
         <v>78.643000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>70.647999999999996</v>
       </c>
@@ -492,7 +490,7 @@
         <v>64.099999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>74.796000000000006</v>
       </c>
@@ -512,7 +510,7 @@
         <v>68.704999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>71.375</v>
       </c>
@@ -532,7 +530,7 @@
         <v>62.656999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>64.974999999999994</v>
       </c>
@@ -552,7 +550,7 @@
         <v>61.74</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>66.626999999999995</v>
       </c>
@@ -572,7 +570,7 @@
         <v>72.393000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>80.582999999999998</v>
       </c>
@@ -592,7 +590,7 @@
         <v>69.257999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>74.978999999999999</v>
       </c>
@@ -612,7 +610,7 @@
         <v>81.558999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>61.009</v>
       </c>
@@ -632,7 +630,7 @@
         <v>71.570999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>67.685000000000002</v>
       </c>
@@ -652,7 +650,7 @@
         <v>76.44</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>69.506</v>
       </c>
@@ -672,7 +670,7 @@
         <v>78.182000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>68.974999999999994</v>
       </c>
@@ -692,7 +690,7 @@
         <v>68.733999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>63.194000000000003</v>
       </c>
@@ -712,7 +710,7 @@
         <v>80.048000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>67.643000000000001</v>
       </c>
@@ -732,7 +730,7 @@
         <v>75.179000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>77.474000000000004</v>
       </c>
@@ -752,7 +750,7 @@
         <v>76.260999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>62.284999999999997</v>
       </c>
@@ -772,7 +770,7 @@
         <v>60.895000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>72.174999999999997</v>
       </c>
@@ -792,7 +790,7 @@
         <v>63.384999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>77.960999999999999</v>
       </c>
@@ -812,7 +810,7 @@
         <v>76.349999999999994</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>71.537000000000006</v>
       </c>

</xml_diff>